<commit_message>
Enable visualization of results; Minor adjustments
</commit_message>
<xml_diff>
--- a/ptx_now/base_settings.xlsx
+++ b/ptx_now/base_settings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>value</t>
   </si>
@@ -43,25 +43,31 @@
     <t>solver</t>
   </si>
   <si>
+    <t>path_visualization</t>
+  </si>
+  <si>
     <t>C:/Users/mt5285/ptx_data/data/</t>
   </si>
   <si>
-    <t>C:/Users/mt5285/ptx_data/settings/Settings_Duba.xlsx</t>
-  </si>
-  <si>
-    <t>custom</t>
+    <t>C:/Users/mt5285/ptx_data/settings/test.xlsx</t>
+  </si>
+  <si>
+    <t>visualize_only</t>
   </si>
   <si>
     <t>C:/Users/mt5285/ptx_data/results/</t>
   </si>
   <si>
-    <t>C:/Users/mt5285/ptx_data/optimize/</t>
+    <t>C:/Users/mt5285/ptx_data/settings/porsche/</t>
   </si>
   <si>
     <t>C:/Users/mt5285/ptx_data/settings/</t>
   </si>
   <si>
     <t>gurobi</t>
+  </si>
+  <si>
+    <t>C:/Users/mt5285/ptx_data/results/20211220_093208_test/</t>
   </si>
 </sst>
 </file>
@@ -419,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -438,7 +444,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -446,7 +452,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -454,7 +460,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -462,7 +468,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -470,7 +476,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -478,7 +484,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -486,7 +492,15 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>